<commit_message>
Dokumentation erweitert und Berechnung in Excel zu Längspressverband verbessert
</commit_message>
<xml_diff>
--- a/Längspressverband_Auslegungsmoment.xlsx
+++ b/Längspressverband_Auslegungsmoment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hofmannt.tmb18\Documents\GitHub\KE4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF26D15E-A86D-4255-86A2-CCB50E4761AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521F2DE3-33FC-4C70-B547-5E651A52F384}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" tabRatio="345" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" tabRatio="345" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="09-pressv20" sheetId="1" r:id="rId1"/>
@@ -3370,8 +3370,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3392,7 +3392,7 @@
       </c>
       <c r="D1" s="12">
         <f ca="1">NOW()</f>
-        <v>43852.626130555553</v>
+        <v>43852.710509606484</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3613,7 +3613,7 @@
         <v>18</v>
       </c>
       <c r="D27" s="23">
-        <v>20</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -3625,7 +3625,7 @@
         <v>20</v>
       </c>
       <c r="D28" s="23">
-        <v>242.5</v>
+        <v>268</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3798,7 +3798,7 @@
       </c>
       <c r="D44" s="25">
         <f>D26/D28</f>
-        <v>0.89484536082474231</v>
+        <v>0.80970149253731338</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -3822,7 +3822,7 @@
       </c>
       <c r="D46" s="25">
         <f>D35/D36*((1+D45^2)/(1-D45^2)-D38)+(1+D44^2)/(1-D44^2)+D37</f>
-        <v>10.037551473255245</v>
+        <v>5.8074792803719406</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="D50" s="25">
         <f>IF(AND(D45=0,D35=D36,D37=D38),D49*10^-3*((1-D44^2)/2)*D35,D49*10^-3*D35/D46)</f>
-        <v>32.298070824433701</v>
+        <v>55.823453298026017</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -3887,7 +3887,7 @@
       </c>
       <c r="D51" s="29">
         <f>D50*D26*PI()*D27*D23</f>
-        <v>79266.318839620319</v>
+        <v>119877.27418504797</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -3900,7 +3900,7 @@
       </c>
       <c r="D52" s="30">
         <f>D51/D22</f>
-        <v>39633.159419810159</v>
+        <v>59938.637092523983</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3913,7 +3913,7 @@
       </c>
       <c r="D53" s="31">
         <f>D52*(D26*10^-3/2)</f>
-        <v>4300.1977970494027</v>
+        <v>6503.3421245388517</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3926,7 +3926,7 @@
       </c>
       <c r="D54" s="29">
         <f>D52</f>
-        <v>39633.159419810159</v>
+        <v>59938.637092523983</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -3981,7 +3981,7 @@
       </c>
       <c r="D59" s="31">
         <f>IF(AND(D45=0,D35=D36,D37=D38),D58*10^-3*((1-D44^2)/2)*D35,D58*10^-3*D35/D46)</f>
-        <v>39.528982203038261</v>
+        <v>68.321241349822898</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -3994,7 +3994,7 @@
       </c>
       <c r="D60" s="34">
         <f>(1-D44^2)/(SQRT(3)*D24)*D39</f>
-        <v>71.898793088129892</v>
+        <v>124.26868898631899</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -4076,8 +4076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2F864B-7449-46FD-ADE2-616EB2F8A424}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4098,7 +4098,7 @@
       </c>
       <c r="D1" s="12">
         <f ca="1">NOW()</f>
-        <v>43852.626130555553</v>
+        <v>43852.710509606484</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4781,8 +4781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149A42DD-EE91-4D0C-A349-96B11DB8A54E}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4803,7 +4803,7 @@
       </c>
       <c r="D1" s="12">
         <f ca="1">NOW()</f>
-        <v>43852.626130555553</v>
+        <v>43852.710509606484</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5036,7 +5036,7 @@
         <v>20</v>
       </c>
       <c r="D28" s="23">
-        <v>264.60000000000002</v>
+        <v>310.2</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5209,7 +5209,7 @@
       </c>
       <c r="D44" s="25">
         <f>D26/D28</f>
-        <v>0.82010582010582</v>
+        <v>0.69954867827208256</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -5233,7 +5233,7 @@
       </c>
       <c r="D46" s="25">
         <f>D35/D36*((1+D45^2)/(1-D45^2)-D38)+(1+D44^2)/(1-D44^2)+D37</f>
-        <v>6.1082421340629258</v>
+        <v>3.9167176825336876</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -5285,7 +5285,7 @@
       </c>
       <c r="D50" s="25">
         <f>IF(AND(D45=0,D35=D36,D37=D38),D49*10^-3*((1-D44^2)/2)*D35,D49*10^-3*D35/D46)</f>
-        <v>53.074770330274703</v>
+        <v>82.771742735713104</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -5298,7 +5298,7 @@
       </c>
       <c r="D51" s="29">
         <f>D50*D26*PI()*D27*D23</f>
-        <v>146538.84132844509</v>
+        <v>228531.84667120088</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -5311,7 +5311,7 @@
       </c>
       <c r="D52" s="30">
         <f>D51/D22</f>
-        <v>73269.420664222547</v>
+        <v>114265.92333560044</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5324,7 +5324,7 @@
       </c>
       <c r="D53" s="31">
         <f>D52*(D26*10^-3/2)</f>
-        <v>7949.7321420681465</v>
+        <v>12397.852681912647</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5337,7 +5337,7 @@
       </c>
       <c r="D54" s="29">
         <f>D52</f>
-        <v>73269.420664222547</v>
+        <v>114265.92333560044</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -5392,7 +5392,7 @@
       </c>
       <c r="D59" s="31">
         <f>IF(AND(D45=0,D35=D36,D37=D38),D58*10^-3*((1-D44^2)/2)*D35,D58*10^-3*D35/D46)</f>
-        <v>64.957181598246649</v>
+        <v>101.30272991535035</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -5405,7 +5405,7 @@
       </c>
       <c r="D60" s="34">
         <f>(1-D44^2)/(SQRT(3)*D24)*D39</f>
-        <v>118.14984092763825</v>
+        <v>184.25832418439188</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -5486,8 +5486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A652CE9-BA66-4652-B792-720AED5D7E82}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5508,7 +5508,7 @@
       </c>
       <c r="D1" s="12">
         <f ca="1">NOW()</f>
-        <v>43852.626130555553</v>
+        <v>43852.710509606484</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5741,7 +5741,7 @@
         <v>20</v>
       </c>
       <c r="D28" s="23">
-        <v>246</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5914,7 +5914,7 @@
       </c>
       <c r="D44" s="25">
         <f>D26/D28</f>
-        <v>0.88211382113821135</v>
+        <v>0.78909090909090907</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -5938,7 +5938,7 @@
       </c>
       <c r="D46" s="25">
         <f>D35/D36*((1+D45^2)/(1-D45^2)-D38)+(1+D44^2)/(1-D44^2)+D37</f>
-        <v>9.0140761152900826</v>
+        <v>5.3003223997757214</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -5990,7 +5990,7 @@
       </c>
       <c r="D50" s="25">
         <f>IF(AND(D45=0,D35=D36,D37=D38),D49*10^-3*((1-D44^2)/2)*D35,D49*10^-3*D35/D46)</f>
-        <v>35.965255256407815</v>
+        <v>61.164873367102125</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -6003,7 +6003,7 @@
       </c>
       <c r="D51" s="29">
         <f>D50*D26*PI()*D27*D23</f>
-        <v>176532.7350849747</v>
+        <v>300223.1545318141</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -6016,7 +6016,7 @@
       </c>
       <c r="D52" s="30">
         <f>D51/D22</f>
-        <v>88266.367542487351</v>
+        <v>150111.57726590705</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6029,7 +6029,7 @@
       </c>
       <c r="D53" s="31">
         <f>D52*(D26*10^-3/2)</f>
-        <v>9576.9008783598783</v>
+        <v>16287.106133350915</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6042,7 +6042,7 @@
       </c>
       <c r="D54" s="29">
         <f>D52</f>
-        <v>88266.367542487351</v>
+        <v>150111.57726590705</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -6097,7 +6097,7 @@
       </c>
       <c r="D59" s="31">
         <f>IF(AND(D45=0,D35=D36,D37=D38),D58*10^-3*((1-D44^2)/2)*D35,D58*10^-3*D35/D46)</f>
-        <v>44.017178075006576</v>
+        <v>74.858501732871247</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -6110,7 +6110,7 @@
       </c>
       <c r="D60" s="34">
         <f>(1-D44^2)/(SQRT(3)*D24)*D39</f>
-        <v>80.06231889509705</v>
+        <v>136.15923373219147</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -6191,8 +6191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5AC2237-01B7-47E0-9D9E-AB3E32901ED8}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="B1" s="37">
         <f>'09-pressv20'!D51+'09-pressv20 (2)'!D51+'09-pressv20 (3)'!D51+'09-pressv20 (4)'!D51</f>
-        <v>918002.34243826254</v>
+        <v>1164296.7225732855</v>
       </c>
       <c r="C1" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
Doku zu Pressverbindung fertig gestellt, Fehler in Excel ausgebessert
</commit_message>
<xml_diff>
--- a/Längspressverband_Auslegungsmoment.xlsx
+++ b/Längspressverband_Auslegungsmoment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hofmannt.tmb18\Documents\GitHub\KE4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521F2DE3-33FC-4C70-B547-5E651A52F384}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FAC585-D250-4617-8AE3-C490163B02CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" tabRatio="345" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" tabRatio="345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="09-pressv20" sheetId="1" r:id="rId1"/>
@@ -3370,7 +3370,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -3392,7 +3392,7 @@
       </c>
       <c r="D1" s="12">
         <f ca="1">NOW()</f>
-        <v>43852.710509606484</v>
+        <v>43858.525868518518</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3749,7 +3749,8 @@
         <v>30</v>
       </c>
       <c r="D39" s="23">
-        <v>750</v>
+        <f>750*0.9</f>
+        <v>675</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3994,7 +3995,7 @@
       </c>
       <c r="D60" s="34">
         <f>(1-D44^2)/(SQRT(3)*D24)*D39</f>
-        <v>124.26868898631899</v>
+        <v>111.84182008768708</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -4076,8 +4077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2F864B-7449-46FD-ADE2-616EB2F8A424}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4098,7 +4099,7 @@
       </c>
       <c r="D1" s="12">
         <f ca="1">NOW()</f>
-        <v>43852.710509606484</v>
+        <v>43858.525868518518</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4455,7 +4456,8 @@
         <v>30</v>
       </c>
       <c r="D39" s="23">
-        <v>750</v>
+        <f>750*0.9</f>
+        <v>675</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4700,7 +4702,7 @@
       </c>
       <c r="D60" s="34">
         <f>(1-D44^2)/(SQRT(3)*D24)*D39</f>
-        <v>311.82349942847242</v>
+        <v>280.64114948562519</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -4781,8 +4783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149A42DD-EE91-4D0C-A349-96B11DB8A54E}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4803,7 +4805,7 @@
       </c>
       <c r="D1" s="12">
         <f ca="1">NOW()</f>
-        <v>43852.710509606484</v>
+        <v>43858.525868518518</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5160,7 +5162,8 @@
         <v>30</v>
       </c>
       <c r="D39" s="23">
-        <v>750</v>
+        <f>750*0.9</f>
+        <v>675</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5405,7 +5408,7 @@
       </c>
       <c r="D60" s="34">
         <f>(1-D44^2)/(SQRT(3)*D24)*D39</f>
-        <v>184.25832418439188</v>
+        <v>165.83249176595271</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -5487,7 +5490,7 @@
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5508,7 +5511,7 @@
       </c>
       <c r="D1" s="12">
         <f ca="1">NOW()</f>
-        <v>43852.710509606484</v>
+        <v>43858.525868518518</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5865,7 +5868,8 @@
         <v>30</v>
       </c>
       <c r="D39" s="23">
-        <v>750</v>
+        <f>750*0.9</f>
+        <v>675</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -6110,7 +6114,7 @@
       </c>
       <c r="D60" s="34">
         <f>(1-D44^2)/(SQRT(3)*D24)*D39</f>
-        <v>136.15923373219147</v>
+        <v>122.54331035897231</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
@@ -6191,8 +6195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5AC2237-01B7-47E0-9D9E-AB3E32901ED8}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>